<commit_message>
Rettet noget tekst i backlog
</commit_message>
<xml_diff>
--- a/Product backlog.xlsx
+++ b/Product backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18780" windowHeight="21000" tabRatio="500"/>
+    <workbookView xWindow="2400" yWindow="460" windowWidth="18780" windowHeight="19500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>godkendelse</t>
   </si>
   <si>
-    <t>Tegning bliver oprettet til brug for godkendelse ifht. Hvad kunden har bestilt</t>
-  </si>
-  <si>
     <t>Godkendelse af kommune</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>Mellem</t>
+  </si>
+  <si>
+    <t>Tegning bliver oprettet med kundens dimensioner til brug for godkendelse hos kommunen.</t>
   </si>
 </sst>
 </file>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,28 +523,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H1" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -552,10 +552,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -566,7 +566,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -574,10 +574,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
@@ -588,7 +588,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -596,10 +596,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>1</v>
@@ -610,7 +610,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -618,13 +618,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>3</v>
@@ -632,7 +632,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -640,13 +640,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>6</v>
@@ -654,7 +654,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -662,21 +662,21 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -684,21 +684,21 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -706,21 +706,21 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -728,21 +728,21 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -750,21 +750,21 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="80" x14ac:dyDescent="0.2">
@@ -772,21 +772,21 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>